<commit_message>
changed the Excel login and register methods
</commit_message>
<xml_diff>
--- a/BirdManagementSystem/Users.xlsx
+++ b/BirdManagementSystem/Users.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LasTa\Desktop\BirdsProject\BirdProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lidor\source\repos\BirdManagementSystem\BirdManagementSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59559FA6-A43A-42F7-B2DC-C876745582A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5688B486-4484-49E6-BC2E-202EAF6FDD32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D89701BE-4EBE-40EB-8165-8427D0CFFC88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -33,25 +44,39 @@
     <t>Password</t>
   </si>
   <si>
-    <t>mohamad</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Lidorfel</t>
+  </si>
+  <si>
+    <t>12345678a@</t>
+  </si>
+  <si>
+    <t>moemoe</t>
   </si>
   <si>
     <t>alonss12A!</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>LidorFEL</t>
+  </si>
+  <si>
+    <t>209297035</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
+      <charset val="177"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -75,9 +100,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -96,7 +120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -112,7 +136,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -124,7 +148,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -171,6 +195,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -206,6 +247,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -357,129 +415,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BFDF9D-3478-4BAC-ACBF-4686658E0978}">
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="11.69921875" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="9.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="0">
+        <v>209297035</v>
+      </c>
     </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="0">
+        <v>213169914</v>
       </c>
     </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="11">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="12">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="13">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="14">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="15">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row spans="1:3" x14ac:dyDescent="0.3" outlineLevel="0" r="16">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row outlineLevel="0" r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>moemoe</t>
-        </is>
-      </c>
-      <c r="B17" s="1" t="inlineStr">
-        <is>
-          <t>alonss12A!</t>
-        </is>
-      </c>
-      <c r="C17" s="1" t="inlineStr">
-        <is>
-          <t>213169914</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Lidorfel</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>12345678a@</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>209297035</t>
-        </is>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>